<commit_message>
Changed the view so the video isn't as bulky and is off to the side
</commit_message>
<xml_diff>
--- a/files/books.xlsx
+++ b/files/books.xlsx
@@ -20,141 +20,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">Book Names</t>
   </si>
   <si>
-    <t xml:space="preserve">Fed-Batch Fermentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyber Reconnaissance, Surveillance and Defense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optimized Cloud Resource Management and Scheduling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Landslide Hazards, Risks, and Disasters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wildfire Hazards, Risks, and Disasters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Storage for Smart Grids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Guide to Oilwell Fishing Operations (Second Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unconventional Gas Reservoirs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palladium Membrane Technology for Hydrogen Production, Carbon Capture and Other Applications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas Turbines (Second Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regulatory Affairs for Biomaterials and Medical Devices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional Finishes for Textiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Learning from the Impacts of Superstorm Sandy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hedge Fund Governance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intelligent Coatings for Corrosion Control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fatigue and Fracture of Adhesively-Bonded Composite Joints</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modelling Degradation of Bioresorbable Polymeric Medical Devices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An Introduction to Probability and Statistical Inference (Second Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designing Plastic Parts for Assembly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaping Knowledge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polyphenols in Plants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key Chiral Auxiliary Applications (Second Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relevance Ranking for Vertical Search Engines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commercial Data Mining</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object-Oriented Analysis and Design for Information Systems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Design Modeling using CAD/CAE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elasticity (Third Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drinking Water Security for Engineers, Planners, and Managers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nuclear Energy (Seventh Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piping and Pipeline Calculations Manual (Second Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomarkers in Toxicology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drug Stability for Pharmaceutical Scientists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polymer Testing (Second Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atlas of Chick Development (Third Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stem Cells (Second Edition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rare Diseases and Orphan Drugs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heterogeneous Catalytic Materials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Braking of Road Vehicles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friction Stir Superplasticity for Unitized Structures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High Performance Silicon Imaging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advanced Composites in Bridge Construction and Repair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensor Technologies for Civil Infrastructures, Volume 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miscarriages of Justice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security Leader Insights for Effective Management</t>
+    <t xml:space="preserve">Santa Paws, Our Hero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Puppy Place, Noodle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kidnapped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Young Americans Colonial Williamsburg Anns Story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic Tricks from the Tree House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some Good News</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Puppet Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dogs in the Dead of Night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I Survived The Bombing of Pearl Harbor, 1941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emilys Runaway Imagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Of A Kind Family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hopscotch Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brave Emily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stink  and the Ultimate Thumb Wrestling Smackdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horrible Harry At Halloween</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Puppy Place, Sweetie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Land of Stories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Out of My Mind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insectlopedia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What Do You Call A Rhyming Riddle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animals Animals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haggis and Tank Unleashed: All Paws On Deck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Im Glad Iim Me. Poems about You</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pippi Longstocking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Little Go Exploring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sounder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blackbird Fly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary Margaret Mary Christmas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Tale of Despereaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Superfudge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramona And Her Father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Girls Take Over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anastasia At This Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double Fudge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junie B. Jones Has a Peep In Her Pocket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Enchanted Castle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operation Clean Sweep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Whimpy Kid Do It Yourself Book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cicada Summer</t>
   </si>
 </sst>
 </file>
@@ -262,25 +253,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A45"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -288,21 +285,33 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -482,21 +491,6 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up code to insert into students and books to the database from an excel file
</commit_message>
<xml_diff>
--- a/files/books.xlsx
+++ b/files/books.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -160,7 +160,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -253,97 +252,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.6173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -358,17 +339,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -378,7 +359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -393,7 +374,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -403,22 +384,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -433,12 +414,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -448,17 +429,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -468,22 +449,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="19.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Added new books to the excel sheet
</commit_message>
<xml_diff>
--- a/files/books.xlsx
+++ b/files/books.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
   <si>
     <t xml:space="preserve">Book Names</t>
   </si>
@@ -146,6 +146,195 @@
   </si>
   <si>
     <t xml:space="preserve">Cicada Summer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twenty and Ten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Quilts Ida Lous Story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I survived the Battle Of Ghettysburg, 1863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huckleberry Fin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grandmas General Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walk Across The Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Magic School Bus, Inside The Human Body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gordon Korman. Why Did the Underwear Cross The Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calender Mysteries March Mischief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Mystery Of the Coon Cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Mysterious Benedict Society and The Prisoners Dilemma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calender Mysteries January Joker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Mystery of the Magis Treasure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girl Meets World, Friend Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The OodleThunks, Oona Finds an Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Puppy Place, Lucky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alices Adventures in Wonderland </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clementines Letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpiderMan Attack of the Heroes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphix goes to school </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Puppy Place, Bear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Series Of Unfortunate Events, The Slippery Slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From Broad Street to Beacon Hill. Rocket Girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Upstairs Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ready Freddy Tooth Troubles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anna on the Farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junie B, First Grader At last</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet Molly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Young Cam Jansen and the Baseball Mystery </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet Addy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy Birthday, Kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The First Thanksgiving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop Everything, its D.E.A.R Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Indian In The Cupboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 Birthdays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judy Moody The Doctor Is In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judy Moody Declares Independence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dog Man Unleashed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presenting, Talulah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ive Got A Secret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junie B. First Grader. Boss Of Lunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letting Swift River Go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Louisiana Sky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encyclopedia Brown. Everyones Favorite Boy Detective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heidi Heckelbeck Has A Secret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Summer of the Swans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beverly Cleary Henry and Beezus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Babysitters Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mountian Born</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Behind The Mountains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom Sayer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the Banks of Plum Creek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Story of Harriett Tubman. Freedom Train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All The Way Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Hero Two Doors Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looniverse. Stage Freight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riding Freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Little Princess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Race The Wild. Rain Forest Relay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eyes On Nature Spiders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinosaur Bites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghosts</t>
   </si>
 </sst>
 </file>
@@ -155,11 +344,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -175,6 +365,87 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -183,16 +454,64 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -200,8 +519,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,25 +559,153 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -252,16 +714,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A42"/>
+  <dimension ref="A1:A106"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A75" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,10 +936,330 @@
         <v>41</v>
       </c>
     </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added books to the file
</commit_message>
<xml_diff>
--- a/files/books.xlsx
+++ b/files/books.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
   <si>
     <t xml:space="preserve">Book Names</t>
   </si>
@@ -335,6 +335,105 @@
   </si>
   <si>
     <t xml:space="preserve">Ghosts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">----------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extreme Sports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little Bear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth Science and Weather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crocodile Encounters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grimmtastic Girls Sleeping Beauty Dreams Big</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Bear Called Paddington</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giant Dinosaurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calendar Mysteries February Friend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Yellow House Mystery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Den A Tree A Nest Is Best</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Underground Railroad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nancy Drew The Secret Lost At Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Gift Of Heritage Historic Blacks in the Arts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Gift Of Heritage Historic Black Firsts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Wind in the Willows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philip Hall Likes Me I Reckon Maybe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aliens Dont Carve Jack O Lanterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Giraffe and the Pelly and Me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Election Day Disaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pete the Cat And His Four Groovy Buttons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Land of Many Colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploring Planets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Focus on Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chito Rodriguez-Gomez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZooBooks Wolves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thirteen Moons On Turtles Back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cordelia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shapes in the Sky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Rainbow All Around Me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploring Weather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If You Were A Minute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flakes and Fluries</t>
   </si>
 </sst>
 </file>
@@ -714,10 +813,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A106"/>
+  <dimension ref="A1:A140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A75" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A107" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A107" activeCellId="0" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1256,6 +1355,176 @@
         <v>104</v>
       </c>
     </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>